<commit_message>
Project folder cleanup for release with thesis
Removed files related to IAPMEI
Reduced the number of files generated throughout the modeling phase, containing only the final ones
Removed files related to XAI models that were not implemented
IAPMEI Jupyter notebooks still missing, to be added later
</commit_message>
<xml_diff>
--- a/German Credit Tables.xlsx
+++ b/German Credit Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rhinestein\Documents\ISCTE\Código Tese\thesis_mcd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6BFEFE7-25EF-42F4-8876-6346AD75A9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C696F8E-3811-41C8-BC94-07733FC7E710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B667C264-0C63-407B-AFF1-EAC0CE29D1D2}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>Feature</t>
   </si>
@@ -120,14 +120,154 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Credit history_all_paid_duly</t>
+  </si>
+  <si>
+    <t>Credit history_critical</t>
+  </si>
+  <si>
+    <t>Credit history_delay</t>
+  </si>
+  <si>
+    <t>Credit history_existing_duly_until_now</t>
+  </si>
+  <si>
+    <t>Credit history_none_paid_duly</t>
+  </si>
+  <si>
+    <t>Purpose_business</t>
+  </si>
+  <si>
+    <t>Purpose_car_new</t>
+  </si>
+  <si>
+    <t>Purpose_car_used</t>
+  </si>
+  <si>
+    <t>Purpose_domestic_appliances</t>
+  </si>
+  <si>
+    <t>Purpose_education</t>
+  </si>
+  <si>
+    <t>Purpose_furniture_equipment</t>
+  </si>
+  <si>
+    <t>Purpose_others</t>
+  </si>
+  <si>
+    <t>Purpose_radio_television</t>
+  </si>
+  <si>
+    <t>Purpose_repairs</t>
+  </si>
+  <si>
+    <t>Purpose_retraining</t>
+  </si>
+  <si>
+    <t>Personal status and sex_female_divorced_separated_married</t>
+  </si>
+  <si>
+    <t>Personal status and sex_male_divorced_separated</t>
+  </si>
+  <si>
+    <t>Personal status and sex_male_married_widowed</t>
+  </si>
+  <si>
+    <t>Personal status and sex_male_single</t>
+  </si>
+  <si>
+    <t>Other debtors or guarantors_coapplicant</t>
+  </si>
+  <si>
+    <t>Other debtors or guarantors_guarantor</t>
+  </si>
+  <si>
+    <t>Other debtors or guarantors_none</t>
+  </si>
+  <si>
+    <t>Property_car_other</t>
+  </si>
+  <si>
+    <t>Property_real estate</t>
+  </si>
+  <si>
+    <t>Property_soc_savings_life_insurance</t>
+  </si>
+  <si>
+    <t>Property_unknown</t>
+  </si>
+  <si>
+    <t>Other installment plans_bank</t>
+  </si>
+  <si>
+    <t>Other installment plans_none</t>
+  </si>
+  <si>
+    <t>Other installment plans_stores</t>
+  </si>
+  <si>
+    <t>Housing_free</t>
+  </si>
+  <si>
+    <t>Housing_own</t>
+  </si>
+  <si>
+    <t>Housing_rent</t>
+  </si>
+  <si>
+    <t>Telephone_none</t>
+  </si>
+  <si>
+    <t>Telephone_yes</t>
+  </si>
+  <si>
+    <t>Foreign worker_no</t>
+  </si>
+  <si>
+    <t>Foreign worker_yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -143,7 +283,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,13 +291,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35334B26-84DC-4609-91FE-BC9A7F7E2E48}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="K1" sqref="K1:S49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +643,7 @@
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,8 +671,32 @@
       <c r="I1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -542,8 +724,35 @@
       <c r="I2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>862</v>
+      </c>
+      <c r="M2">
+        <v>0.54021655065738583</v>
+      </c>
+      <c r="N2">
+        <v>0.42245532761712828</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -571,8 +780,35 @@
       <c r="I3">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>862</v>
+      </c>
+      <c r="M3">
+        <v>0.37147392844059091</v>
+      </c>
+      <c r="N3">
+        <v>0.22868603412280289</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0.21052631578947359</v>
+      </c>
+      <c r="Q3">
+        <v>0.36842105263157893</v>
+      </c>
+      <c r="R3">
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -600,8 +836,35 @@
       <c r="I4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>862</v>
+      </c>
+      <c r="M4">
+        <v>0.29892986302635871</v>
+      </c>
+      <c r="N4">
+        <v>0.2179805830955471</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0.13865959119496851</v>
+      </c>
+      <c r="Q4">
+        <v>0.23801100628930821</v>
+      </c>
+      <c r="R4">
+        <v>0.40683962264150941</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -629,8 +892,35 @@
       <c r="I5">
         <v>184</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>862</v>
+      </c>
+      <c r="M5">
+        <v>0.30510440835266822</v>
+      </c>
+      <c r="N5">
+        <v>0.24606671381161949</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0.25</v>
+      </c>
+      <c r="Q5">
+        <v>0.25</v>
+      </c>
+      <c r="R5">
+        <v>0.25</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -658,8 +948,35 @@
       <c r="I6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <v>862</v>
+      </c>
+      <c r="M6">
+        <v>0.59831786542923437</v>
+      </c>
+      <c r="N6">
+        <v>0.29779495651613852</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0.5</v>
+      </c>
+      <c r="Q6">
+        <v>0.5</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -687,8 +1004,35 @@
       <c r="I7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>862</v>
+      </c>
+      <c r="M7">
+        <v>0.67246713070378972</v>
+      </c>
+      <c r="N7">
+        <v>0.36928446070767812</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Q7">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -716,8 +1060,35 @@
       <c r="I8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8">
+        <v>862</v>
+      </c>
+      <c r="M8">
+        <v>0.60788863109048719</v>
+      </c>
+      <c r="N8">
+        <v>0.36796434145853341</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Q8">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -745,8 +1116,35 @@
       <c r="I9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9">
+        <v>862</v>
+      </c>
+      <c r="M9">
+        <v>0.34885279711265788</v>
+      </c>
+      <c r="N9">
+        <v>0.22810584852163779</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0.1777777777777777</v>
+      </c>
+      <c r="Q9">
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="R9">
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -774,8 +1172,35 @@
       <c r="I10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10">
+        <v>862</v>
+      </c>
+      <c r="M10">
+        <v>0.13263727764887859</v>
+      </c>
+      <c r="N10">
+        <v>0.1882180161137422</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -803,8 +1228,35 @@
       <c r="I11">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11">
+        <v>862</v>
+      </c>
+      <c r="M11">
+        <v>0.62219644238205729</v>
+      </c>
+      <c r="N11">
+        <v>0.20750463058759311</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="Q11">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="R11">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -832,8 +1284,35 @@
       <c r="I12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12">
+        <v>862</v>
+      </c>
+      <c r="M12">
+        <v>0.1531322505800464</v>
+      </c>
+      <c r="N12">
+        <v>0.36032399751658789</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -861,8 +1340,35 @@
       <c r="I13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13">
+        <v>862</v>
+      </c>
+      <c r="M13">
+        <v>0.26450116009280739</v>
+      </c>
+      <c r="N13">
+        <v>0.44132328662826431</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -890,8 +1396,35 @@
       <c r="I14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14">
+        <v>862</v>
+      </c>
+      <c r="M14">
+        <v>4.7563805104408351E-2</v>
+      </c>
+      <c r="N14">
+        <v>0.21296503121131749</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -919,8 +1452,35 @@
       <c r="I15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15">
+        <v>862</v>
+      </c>
+      <c r="M15">
+        <v>0.30046403712296982</v>
+      </c>
+      <c r="N15">
+        <v>0.4587259718919473</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -948,8 +1508,35 @@
       <c r="I16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16">
+        <v>862</v>
+      </c>
+      <c r="M16">
+        <v>7.8886310904872387E-2</v>
+      </c>
+      <c r="N16">
+        <v>0.26971773187516551</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -977,8 +1564,35 @@
       <c r="I17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17">
+        <v>862</v>
+      </c>
+      <c r="M17">
+        <v>0.54060324825986084</v>
+      </c>
+      <c r="N17">
+        <v>0.49863796636368329</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1006,8 +1620,35 @@
       <c r="I18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18">
+        <v>862</v>
+      </c>
+      <c r="M18">
+        <v>3.248259860788863E-2</v>
+      </c>
+      <c r="N18">
+        <v>0.1773808911159164</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1035,8 +1676,35 @@
       <c r="I19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19">
+        <v>862</v>
+      </c>
+      <c r="M19">
+        <v>8.2366589327146175E-2</v>
+      </c>
+      <c r="N19">
+        <v>0.27508202167743251</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1064,8 +1732,35 @@
       <c r="I20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20">
+        <v>862</v>
+      </c>
+      <c r="M20">
+        <v>0.23781902552204179</v>
+      </c>
+      <c r="N20">
+        <v>0.42599490676531487</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1093,8 +1788,35 @@
       <c r="I21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21">
+        <v>862</v>
+      </c>
+      <c r="M21">
+        <v>8.4686774941995363E-2</v>
+      </c>
+      <c r="N21">
+        <v>0.2785766573870152</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1120,6 +1842,816 @@
         <v>1</v>
       </c>
       <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22">
+        <v>862</v>
+      </c>
+      <c r="M22">
+        <v>1.276102088167053E-2</v>
+      </c>
+      <c r="N22">
+        <v>0.1123067640751382</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23">
+        <v>862</v>
+      </c>
+      <c r="M23">
+        <v>4.6403712296983757E-2</v>
+      </c>
+      <c r="N23">
+        <v>0.21047993249685321</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L24">
+        <v>862</v>
+      </c>
+      <c r="M24">
+        <v>0.20185614849187941</v>
+      </c>
+      <c r="N24">
+        <v>0.40161843050264739</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25">
+        <v>862</v>
+      </c>
+      <c r="M25">
+        <v>5.8004640371229696E-3</v>
+      </c>
+      <c r="N25">
+        <v>7.5983659223587213E-2</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L26">
+        <v>862</v>
+      </c>
+      <c r="M26">
+        <v>0.29582366589327153</v>
+      </c>
+      <c r="N26">
+        <v>0.4566770922077128</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L27">
+        <v>862</v>
+      </c>
+      <c r="M27">
+        <v>2.2041763341067281E-2</v>
+      </c>
+      <c r="N27">
+        <v>0.14690459463975711</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L28">
+        <v>862</v>
+      </c>
+      <c r="M28">
+        <v>1.044083526682135E-2</v>
+      </c>
+      <c r="N28">
+        <v>0.1017045919396026</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29">
+        <v>862</v>
+      </c>
+      <c r="M29">
+        <v>0.3225058004640371</v>
+      </c>
+      <c r="N29">
+        <v>0.46770672321899381</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L30">
+        <v>862</v>
+      </c>
+      <c r="M30">
+        <v>4.9883990719257539E-2</v>
+      </c>
+      <c r="N30">
+        <v>0.21783164443743491</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L31">
+        <v>862</v>
+      </c>
+      <c r="M31">
+        <v>0.10324825986078889</v>
+      </c>
+      <c r="N31">
+        <v>0.30445950828686841</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L32">
+        <v>862</v>
+      </c>
+      <c r="M32">
+        <v>0.52436194895591648</v>
+      </c>
+      <c r="N32">
+        <v>0.49969607379834807</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33">
+        <v>862</v>
+      </c>
+      <c r="M33">
+        <v>3.8283062645011599E-2</v>
+      </c>
+      <c r="N33">
+        <v>0.19199018477111979</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L34">
+        <v>862</v>
+      </c>
+      <c r="M34">
+        <v>5.6844547563805102E-2</v>
+      </c>
+      <c r="N34">
+        <v>0.2316797650924213</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L35">
+        <v>862</v>
+      </c>
+      <c r="M35">
+        <v>0.90487238979118334</v>
+      </c>
+      <c r="N35">
+        <v>0.29356144644223042</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="R35">
+        <v>1</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L36">
+        <v>862</v>
+      </c>
+      <c r="M36">
+        <v>0.32830626450116013</v>
+      </c>
+      <c r="N36">
+        <v>0.46986953874988657</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L37">
+        <v>862</v>
+      </c>
+      <c r="M37">
+        <v>0.30626450116009279</v>
+      </c>
+      <c r="N37">
+        <v>0.46120854684850088</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L38">
+        <v>862</v>
+      </c>
+      <c r="M38">
+        <v>0.24825986078886311</v>
+      </c>
+      <c r="N38">
+        <v>0.43225415937160921</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L39">
+        <v>862</v>
+      </c>
+      <c r="M39">
+        <v>0.11716937354988401</v>
+      </c>
+      <c r="N39">
+        <v>0.32180871904120939</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L40">
+        <v>862</v>
+      </c>
+      <c r="M40">
+        <v>0.13457076566125289</v>
+      </c>
+      <c r="N40">
+        <v>0.34146264470276172</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L41">
+        <v>862</v>
+      </c>
+      <c r="M41">
+        <v>0.81786542923433869</v>
+      </c>
+      <c r="N41">
+        <v>0.38617946456269919</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K42" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L42">
+        <v>862</v>
+      </c>
+      <c r="M42">
+        <v>4.7563805104408351E-2</v>
+      </c>
+      <c r="N42">
+        <v>0.21296503121131741</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K43" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L43">
+        <v>862</v>
+      </c>
+      <c r="M43">
+        <v>7.5406032482598612E-2</v>
+      </c>
+      <c r="N43">
+        <v>0.26419867205253172</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L44">
+        <v>862</v>
+      </c>
+      <c r="M44">
+        <v>0.73549883990719256</v>
+      </c>
+      <c r="N44">
+        <v>0.44132328662826409</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L45">
+        <v>862</v>
+      </c>
+      <c r="M45">
+        <v>0.1890951276102088</v>
+      </c>
+      <c r="N45">
+        <v>0.39181150241628782</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L46">
+        <v>862</v>
+      </c>
+      <c r="M46">
+        <v>0.62296983758700697</v>
+      </c>
+      <c r="N46">
+        <v>0.48492392834184628</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+      <c r="R46">
+        <v>1</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L47">
+        <v>862</v>
+      </c>
+      <c r="M47">
+        <v>0.37703016241299298</v>
+      </c>
+      <c r="N47">
+        <v>0.48492392834184628</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="S47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K48" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L48">
+        <v>862</v>
+      </c>
+      <c r="M48">
+        <v>3.9443155452436193E-2</v>
+      </c>
+      <c r="N48">
+        <v>0.19475984411856609</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L49">
+        <v>862</v>
+      </c>
+      <c r="M49">
+        <v>0.96055684454756385</v>
+      </c>
+      <c r="N49">
+        <v>0.19475984411856609</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+      <c r="R49">
+        <v>1</v>
+      </c>
+      <c r="S49">
         <v>1</v>
       </c>
     </row>

</xml_diff>